<commit_message>
DSE_FH_SW_029: Updated requierements and planning document with the Sprint 04 activities
</commit_message>
<xml_diff>
--- a/2) Planning/7. Planning_20190405.xlsx
+++ b/2) Planning/7. Planning_20190405.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Diagram" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Windows User</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Scrum Master Lead</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Software Developer Lead</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
@@ -39,9 +97,6 @@
     <t>Planing</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
     <t>FG</t>
   </si>
   <si>
@@ -352,13 +407,16 @@
   </si>
   <si>
     <t xml:space="preserve">DSE_FH_IT&amp;V_006: Document Black box test cases </t>
+  </si>
+  <si>
+    <t>FG/HG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +461,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -560,7 +631,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -599,14 +670,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1534,11 +1599,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="216350080"/>
-        <c:axId val="216351872"/>
+        <c:axId val="215333504"/>
+        <c:axId val="215339392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216350080"/>
+        <c:axId val="215333504"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1560,7 +1625,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216351872"/>
+        <c:crossAx val="215339392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1568,7 +1633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216351872"/>
+        <c:axId val="215339392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43687"/>
@@ -1581,7 +1646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216350080"/>
+        <c:crossAx val="215333504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1937,7 +2002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1945,22 +2010,22 @@
   <sheetData>
     <row r="1" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
+      <c r="C2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1972,12 +2037,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,7 +2077,7 @@
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3">
         <v>43672</v>
@@ -2030,12 +2095,12 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3">
         <v>43673</v>
@@ -2050,15 +2115,15 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
         <v>57</v>
-      </c>
-      <c r="I3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>43673</v>
@@ -2092,7 +2157,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>43676</v>
@@ -2104,12 +2169,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
         <v>43676</v>
@@ -2121,12 +2186,12 @@
         <v>1</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>43676</v>
@@ -2138,12 +2203,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>43677</v>
@@ -2155,12 +2220,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3">
         <v>43677</v>
@@ -2172,12 +2237,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <v>43677</v>
@@ -2188,13 +2253,13 @@
       <c r="E11" s="12">
         <v>1</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>7</v>
+      <c r="F11" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3">
         <v>43677</v>
@@ -2206,12 +2271,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3">
         <v>43677</v>
@@ -2223,12 +2288,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
         <v>43677</v>
@@ -2240,12 +2305,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>43677</v>
@@ -2256,13 +2321,13 @@
       <c r="E15" s="12">
         <v>1</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>7</v>
+      <c r="F15" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
         <v>43677</v>
@@ -2274,12 +2339,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3">
         <v>43678</v>
@@ -2291,12 +2356,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3">
         <v>43678</v>
@@ -2308,12 +2373,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="3">
         <v>43678</v>
@@ -2324,13 +2389,13 @@
       <c r="E19" s="12">
         <v>1</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>7</v>
+      <c r="F19" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="3">
         <v>43678</v>
@@ -2342,12 +2407,12 @@
         <v>1</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3">
         <v>43678</v>
@@ -2359,12 +2424,12 @@
         <v>1</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3">
         <v>43678</v>
@@ -2376,12 +2441,12 @@
         <v>1</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3">
         <v>43679</v>
@@ -2398,7 +2463,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3">
         <v>43679</v>
@@ -2409,13 +2474,13 @@
       <c r="E24" s="12">
         <v>3</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>7</v>
+      <c r="F24" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="3">
         <v>43679</v>
@@ -2426,13 +2491,13 @@
       <c r="E25" s="12">
         <v>3</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>7</v>
+      <c r="F25" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3">
         <v>43680</v>
@@ -2444,12 +2509,12 @@
         <v>1</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3">
         <v>43680</v>
@@ -2461,12 +2526,12 @@
         <v>1</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3">
         <v>43680</v>
@@ -2477,13 +2542,13 @@
       <c r="E28" s="12">
         <v>1</v>
       </c>
-      <c r="F28" s="15" t="s">
-        <v>7</v>
+      <c r="F28" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3">
         <v>43680</v>
@@ -2495,12 +2560,12 @@
         <v>1</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3">
         <v>43681</v>
@@ -2512,12 +2577,12 @@
         <v>1</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="3">
         <v>43681</v>
@@ -2529,12 +2594,12 @@
         <v>1</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="3">
         <v>43681</v>
@@ -2545,13 +2610,13 @@
       <c r="E32" s="12">
         <v>1</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>7</v>
+      <c r="F32" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3">
         <v>43681</v>
@@ -2563,12 +2628,12 @@
         <v>1</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="3">
         <v>43681</v>
@@ -2579,13 +2644,13 @@
       <c r="E34" s="12">
         <v>4</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="3">
         <v>43684</v>
@@ -2597,12 +2662,12 @@
         <v>3</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="3">
         <v>43684</v>
@@ -2614,12 +2679,12 @@
         <v>3</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="3">
         <v>43684</v>
@@ -2631,12 +2696,12 @@
         <v>3</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="3">
         <v>43684</v>
@@ -2648,12 +2713,12 @@
         <v>3</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C39" s="3">
         <v>43684</v>
@@ -2665,12 +2730,12 @@
         <v>3</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="3">
         <v>43684</v>
@@ -2682,12 +2747,12 @@
         <v>3</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C41" s="3">
         <v>43684</v>
@@ -2699,12 +2764,12 @@
         <v>3</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C42" s="3">
         <v>43684</v>
@@ -2716,12 +2781,12 @@
         <v>3</v>
       </c>
       <c r="F42" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C43" s="3">
         <v>43684</v>
@@ -2733,12 +2798,12 @@
         <v>3</v>
       </c>
       <c r="F43" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" s="3">
         <v>43684</v>
@@ -2750,12 +2815,12 @@
         <v>3</v>
       </c>
       <c r="F44" s="26" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" s="3">
         <v>43686</v>
@@ -2766,13 +2831,14 @@
       <c r="E45" s="12">
         <v>1</v>
       </c>
-      <c r="F45" s="28" t="s">
-        <v>7</v>
+      <c r="F45" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2794,347 +2860,347 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="41"/>
+        <v>48</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="D5" s="43" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="46"/>
+        <v>52</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="47"/>
+        <v>53</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="51" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="52"/>
+        <v>54</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="50"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="52"/>
+        <v>58</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="50"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="52"/>
+        <v>59</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="50"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="52"/>
+        <v>61</v>
+      </c>
+      <c r="C12" s="47"/>
+      <c r="D12" s="50"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="52"/>
+        <v>62</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="50"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="52"/>
+        <v>63</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="50"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="52"/>
+        <v>64</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="50"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="52"/>
+        <v>65</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="50"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="52"/>
+        <v>66</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="50"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="52"/>
+        <v>67</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="50"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="52"/>
+        <v>68</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="50"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="52"/>
+        <v>69</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="50"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="52"/>
+        <v>70</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="50"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="52"/>
+        <v>71</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="50"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="52"/>
+        <v>72</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="50"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="52"/>
+        <v>73</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="50"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="52"/>
+        <v>74</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="50"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="52"/>
+        <v>75</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="50"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="52"/>
+        <v>76</v>
+      </c>
+      <c r="C27" s="47"/>
+      <c r="D27" s="50"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="52"/>
+        <v>77</v>
+      </c>
+      <c r="C28" s="47"/>
+      <c r="D28" s="50"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="52"/>
+        <v>78</v>
+      </c>
+      <c r="C29" s="47"/>
+      <c r="D29" s="50"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="52"/>
+        <v>79</v>
+      </c>
+      <c r="C30" s="47"/>
+      <c r="D30" s="50"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="52"/>
+        <v>80</v>
+      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="50"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="52"/>
+        <v>81</v>
+      </c>
+      <c r="C32" s="47"/>
+      <c r="D32" s="50"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="52"/>
+        <v>82</v>
+      </c>
+      <c r="C33" s="47"/>
+      <c r="D33" s="50"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="52"/>
+        <v>83</v>
+      </c>
+      <c r="C34" s="47"/>
+      <c r="D34" s="50"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="52"/>
+        <v>84</v>
+      </c>
+      <c r="C35" s="47"/>
+      <c r="D35" s="50"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="53"/>
+        <v>85</v>
+      </c>
+      <c r="C36" s="48"/>
+      <c r="D36" s="51"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="35"/>
+        <v>88</v>
+      </c>
+      <c r="C38" s="31"/>
+      <c r="D38" s="33"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="35"/>
+        <v>89</v>
+      </c>
+      <c r="C39" s="31"/>
+      <c r="D39" s="33"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="35"/>
+        <v>90</v>
+      </c>
+      <c r="C40" s="31"/>
+      <c r="D40" s="33"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="33"/>
-      <c r="D41" s="35"/>
+        <v>91</v>
+      </c>
+      <c r="C41" s="31"/>
+      <c r="D41" s="33"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="35"/>
+        <v>93</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="33"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="35"/>
+        <v>95</v>
+      </c>
+      <c r="C43" s="31"/>
+      <c r="D43" s="33"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="35"/>
+        <v>96</v>
+      </c>
+      <c r="C44" s="31"/>
+      <c r="D44" s="33"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="35"/>
+        <v>97</v>
+      </c>
+      <c r="C45" s="31"/>
+      <c r="D45" s="33"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="33"/>
-      <c r="D46" s="35"/>
+        <v>98</v>
+      </c>
+      <c r="C46" s="31"/>
+      <c r="D46" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>